<commit_message>
feat: Enhance multer configuration to include file type validation for Excel files
</commit_message>
<xml_diff>
--- a/Files/Municipios.xlsx
+++ b/Files/Municipios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Todo\Documentos\Santiago\3_Trabajo Profesional\Full-Stack-Projects\sceev-project\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15007E1-7027-4EAC-B21E-1516F2EA043C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634AC9A9-33A0-4AA4-819A-BCC5059AA69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="1039">
   <si>
     <t>MEDELLIN</t>
   </si>
@@ -3139,6 +3139,9 @@
   </si>
   <si>
     <t>Nombre</t>
+  </si>
+  <si>
+    <t>ID_Departamento</t>
   </si>
 </sst>
 </file>
@@ -3497,7 +3500,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3505,6 +3510,9 @@
       <c r="A1" t="s">
         <v>1037</v>
       </c>
+      <c r="B1" t="s">
+        <v>1038</v>
+      </c>
     </row>
     <row r="2" spans="1:2" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>